<commit_message>
Feb 01 Social Support Update
</commit_message>
<xml_diff>
--- a/Data/SocialSupport.xlsx
+++ b/Data/SocialSupport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abautist/Dropbox (University of Oregon)/RAPID-EC/Data Management R3/EE_R3 Question Bank/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622BD10C-D4BF-DF45-B564-6AF2376D1D23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B059BC-67AC-034A-9193-D50A9A76DC00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-31580" yWindow="460" windowWidth="28800" windowHeight="16400" xr2:uid="{F291446A-8B5F-B145-9D54-D44DAA4A744B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>Question</t>
   </si>
@@ -175,6 +175,51 @@
     <t>•Emotional support
 •Taking care of other children in the household 
 •Other household responsibilities</t>
+  </si>
+  <si>
+    <r>
+      <t>People sometimes look to others for companionship, assistance, or other types of support. How often is each of the following kinds of support available to you if you need it? Please choose one number that describes how often each kind of support was available to i</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n a typical week prior to the COVID-19 pandemic.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+•	Someone you can count on to listen to you when you need to talk
+•	Someone to give you information to help you understand a situation
+•	Someone to give you good advice about a crisis
+•	Someone to confide in or talk to about yourself or your problems
+•	Someone whose advice you really want
+•	Someone to share your most private worries and fears with
+•	Someone to turn to for suggestions about how to deal with a personal problem
+•	Someone who understands your problems
+•	Someone to help you if you were confined to bed
+•	Someone to take you to the doctor if you needed it
+•	Someone to prepare your meals if you were unable to do it yourself
+•	Someone to help with daily chores if you were sick
+•	Someone who shows you love and affection
+•	Someone to love and make you feel wanted
+•	Someone who hugs you
+•	Someone to have a good time with
+•	Someone to get together with for relaxation
+•	Someone to do something enjoyable with
+•	Someone to do things with to help you get your mind off things</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -575,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{177050F3-616B-3741-BC3E-825DF1FCB6B9}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A5:XFD6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -638,7 +683,7 @@
     </row>
     <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -653,26 +698,29 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="119" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
@@ -681,23 +729,38 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" xr:uid="{B3EA7C5B-FAE8-2C44-B05D-BE4C99EE37EC}"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{B3EA7C5B-FAE8-2C44-B05D-BE4C99EE37EC}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{38FBEECC-AA3A-F945-A52C-C975E0099AE4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>